<commit_message>
Fix path when use application with a shorcut
</commit_message>
<xml_diff>
--- a/test/MD95-2042.xlsx
+++ b/test/MD95-2042.xlsx
@@ -7,14 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Serie Id-1FB8C5DF" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Serie Id-6198B9AF" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Serie Id-1FDB2383" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Serie Id-3B2BB420" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Serie Id-125575B2" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Serie Id-16C67B7D" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Serie Id-E001AEC2" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="INTERPOLATION Id-784A2BB4" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Information" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Serie Id-1FB8C5DF" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Serie Id-6198B9AF" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Serie Id-1FDB2383" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Serie Id-3B2BB420" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Serie Id-125575B2" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Serie Id-16C67B7D" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Serie Id-E001AEC2" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="INTERPOLATION Id-784A2BB4" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -420,6 +421,50 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="60" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Created with PyAnalyseries v5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>This file has been created with PyAnalySeries software.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Do not modify or accordingly with documentation.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2985,7 +3030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -8556,7 +8601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -8640,7 +8685,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>#dbdb8d</t>
+          <t>#2d9edb</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -13919,7 +13964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -20394,7 +20439,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -25965,7 +26010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -25979,7 +26024,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="1" max="1"/>
     <col width="28" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
@@ -34064,7 +34109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -34078,7 +34123,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="1" max="1"/>
     <col width="31" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
@@ -42163,7 +42208,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>